<commit_message>
added chromosome to the tables
</commit_message>
<xml_diff>
--- a/tables_plots/table_hits_snps_covar.xlsx
+++ b/tables_plots/table_hits_snps_covar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>p value</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>chr</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +489,9 @@
       <c r="E2" t="n">
         <v>0.00839816</v>
       </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -509,6 +517,9 @@
       <c r="E3" t="n">
         <v>0.000376629</v>
       </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,6 +545,9 @@
       <c r="E4" t="n">
         <v>0.009964560000000001</v>
       </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -559,6 +573,9 @@
       <c r="E5" t="n">
         <v>9.62151e-07</v>
       </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,6 +601,9 @@
       <c r="E6" t="n">
         <v>0.00204362</v>
       </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -609,6 +629,9 @@
       <c r="E7" t="n">
         <v>3.12991e-20</v>
       </c>
+      <c r="F7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -634,6 +657,9 @@
       <c r="E8" t="n">
         <v>2.920349999999999e-20</v>
       </c>
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -659,6 +685,9 @@
       <c r="E9" t="n">
         <v>0.00759132</v>
       </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -684,6 +713,9 @@
       <c r="E10" t="n">
         <v>1.04545e-06</v>
       </c>
+      <c r="F10" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -709,6 +741,9 @@
       <c r="E11" t="n">
         <v>0.00270429</v>
       </c>
+      <c r="F11" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -734,6 +769,9 @@
       <c r="E12" t="n">
         <v>1.64634e-06</v>
       </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -758,6 +796,9 @@
       </c>
       <c r="E13" t="n">
         <v>0.00299881</v>
+      </c>
+      <c r="F13" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>